<commit_message>
- Update all SSNs to start with a 9 since that implies they are fake - Corrected logic on field check
</commit_message>
<xml_diff>
--- a/tdrs-backend/tdpservice/parsers/test/data/fra.xlsx
+++ b/tdrs-backend/tdpservice/parsers/test/data/fra.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28619"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10309"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B799DDEA-3E38-4FDB-BDC2-F79FE739BE85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlipe/work/repos/tdrs/TANF-app/tdrs-backend/tdpservice/parsers/test/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D39DA05-0531-6C4D-A233-EB6D052666ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34120" yWindow="500" windowWidth="34140" windowHeight="26380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,14 +41,14 @@
     <t># All data below has errors of some sort</t>
   </si>
   <si>
-    <t>44641241A</t>
+    <t>94641241A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -55,7 +60,7 @@
       <sz val="9"/>
       <color theme="1"/>
       <name val="Helvetica"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -81,7 +86,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -421,25 +426,25 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B13"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2">
         <v>202401</v>
       </c>
       <c r="B1" s="2">
-        <v>446412419</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>946412419</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>202401</v>
       </c>
@@ -447,81 +452,81 @@
         <v>995040265</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>202402</v>
       </c>
       <c r="B3" s="2">
-        <v>109360961</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>909360961</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>202402</v>
       </c>
       <c r="B4" s="2">
-        <v>187777434</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>987777434</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>202403</v>
       </c>
       <c r="B5" s="2">
-        <v>473351423</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>973351423</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>202403</v>
       </c>
       <c r="B6" s="2">
-        <v>509175891</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>909175891</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>202403</v>
       </c>
       <c r="B7" s="2">
-        <v>509175891</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>909175891</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>202301</v>
       </c>
       <c r="B10" s="2">
-        <v>865507</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
+        <v>965507</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>202421</v>
       </c>
       <c r="B11" s="2">
-        <v>669005507</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
+        <v>969005507</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>202300</v>
       </c>
       <c r="B12" s="2">
-        <v>669860000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
+        <v>969860000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>202401</v>
       </c>

</xml_diff>